<commit_message>
use this file and readme to see the scope of work
</commit_message>
<xml_diff>
--- a/Milestones.xlsx
+++ b/Milestones.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunny\Desktop\Betty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E413D0-199B-4074-BCB3-D2C319F9E22D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7611E4A4-DC40-432B-A190-5B75578BB52E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3061E5F0-7863-451F-8C41-DAF595B62750}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{3061E5F0-7863-451F-8C41-DAF595B62750}"/>
   </bookViews>
   <sheets>
     <sheet name="Infographic Timeline" sheetId="2" r:id="rId1"/>
     <sheet name="Chart Data" sheetId="1" r:id="rId2"/>
     <sheet name="About" sheetId="3" r:id="rId3"/>
-    <sheet name="Calc_tem_Constrained Foundation" sheetId="9" r:id="rId4"/>
-    <sheet name="Calc_tem_Nonconstrained Foun" sheetId="10" r:id="rId5"/>
-    <sheet name="word template page 1 " sheetId="5" r:id="rId6"/>
-    <sheet name="word template page 2" sheetId="6" r:id="rId7"/>
-    <sheet name="word template page 3" sheetId="7" r:id="rId8"/>
-    <sheet name="word template page 4" sheetId="8" r:id="rId9"/>
-    <sheet name="Chart Data Hidden" sheetId="4" state="hidden" r:id="rId10"/>
+    <sheet name="LTS-6 Loads in excel sheet" sheetId="11" r:id="rId4"/>
+    <sheet name="Calc_tem_Constrained Foundation" sheetId="9" r:id="rId5"/>
+    <sheet name="Calc_tem_Nonconstrained Foun" sheetId="10" r:id="rId6"/>
+    <sheet name="word template page 1 " sheetId="5" r:id="rId7"/>
+    <sheet name="word template page 2" sheetId="6" r:id="rId8"/>
+    <sheet name="word template page 3" sheetId="7" r:id="rId9"/>
+    <sheet name="word template page 4" sheetId="8" r:id="rId10"/>
+    <sheet name="Chart Data Hidden" sheetId="4" state="hidden" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="142">
   <si>
     <t>Date</t>
   </si>
@@ -362,6 +363,123 @@
   </si>
   <si>
     <t>= IF(C26&lt;7,"7'-0 OK","NG")</t>
+  </si>
+  <si>
+    <t>this cell data will be used in word file</t>
+  </si>
+  <si>
+    <t>this is the only sheet take input from the other excel sheet.</t>
+  </si>
+  <si>
+    <t>in this sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell </t>
+  </si>
+  <si>
+    <t>C81</t>
+  </si>
+  <si>
+    <t>C83</t>
+  </si>
+  <si>
+    <t>C85</t>
+  </si>
+  <si>
+    <t>C87</t>
+  </si>
+  <si>
+    <t>C96</t>
+  </si>
+  <si>
+    <t>C198</t>
+  </si>
+  <si>
+    <t>C200</t>
+  </si>
+  <si>
+    <t>C202</t>
+  </si>
+  <si>
+    <t>C204</t>
+  </si>
+  <si>
+    <t>C213</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>STEEL YIELDING STRENGTH</t>
+  </si>
+  <si>
+    <t>SIGN HEIGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIGN THICKNESS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIGN WIDTH </t>
+  </si>
+  <si>
+    <t>SIGN LENGTH</t>
+  </si>
+  <si>
+    <t>BEHIND AREA</t>
+  </si>
+  <si>
+    <t>Calc_template:LTS-6 Loads in excel sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_collected_fieldsnotes: SHEET1: </t>
+  </si>
+  <si>
+    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$B$2</t>
+  </si>
+  <si>
+    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$C$2</t>
+  </si>
+  <si>
+    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$D$2</t>
+  </si>
+  <si>
+    <t>C224</t>
+  </si>
+  <si>
+    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$e$2</t>
+  </si>
+  <si>
+    <t>data_collected_fieldsnotes.xlsx]reportinfo!$F$2</t>
+  </si>
+  <si>
+    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$G$2</t>
+  </si>
+  <si>
+    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$h$2</t>
+  </si>
+  <si>
+    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$I$2</t>
+  </si>
+  <si>
+    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$J$2</t>
+  </si>
+  <si>
+    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$K$2</t>
+  </si>
+  <si>
+    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$M$2</t>
+  </si>
+  <si>
+    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$L$2</t>
+  </si>
+  <si>
+    <t>foundation depth</t>
+  </si>
+  <si>
+    <t>only first sheet: LTS-6 LOADS take input rom data files data_collected_fieldsnotes.xlsx</t>
   </si>
 </sst>
 </file>
@@ -509,7 +627,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -561,11 +679,17 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -693,8 +817,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="349898" y="145791"/>
-          <a:ext cx="10114772" cy="6564085"/>
+          <a:off x="347993" y="143886"/>
+          <a:ext cx="9932008" cy="6548457"/>
           <a:chOff x="349898" y="349898"/>
           <a:chExt cx="10114772" cy="6564085"/>
         </a:xfrm>
@@ -3210,7 +3334,7 @@
                         <a:latin typeface="Franklin Gothic Book"/>
                       </a:rPr>
                       <a:pPr algn="ctr"/>
-                      <a:t>8 Mar</a:t>
+                      <a:t>9 Mar</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" sz="1200">
                       <a:solidFill>
@@ -3519,7 +3643,7 @@
                         <a:latin typeface="Franklin Gothic Book"/>
                       </a:rPr>
                       <a:pPr algn="ctr"/>
-                      <a:t>11 Mar</a:t>
+                      <a:t>12 Mar</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" sz="1300">
                       <a:solidFill>
@@ -3825,7 +3949,7 @@
                         <a:latin typeface="Franklin Gothic Book"/>
                       </a:rPr>
                       <a:pPr algn="ctr"/>
-                      <a:t>14 Mar</a:t>
+                      <a:t>15 Mar</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" sz="1500">
                       <a:solidFill>
@@ -4131,7 +4255,7 @@
                         <a:latin typeface="Franklin Gothic Book"/>
                       </a:rPr>
                       <a:pPr algn="ctr"/>
-                      <a:t>17 Mar</a:t>
+                      <a:t>18 Mar</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" sz="1500">
                       <a:solidFill>
@@ -4437,7 +4561,7 @@
                         <a:latin typeface="Franklin Gothic Book"/>
                       </a:rPr>
                       <a:pPr algn="ctr"/>
-                      <a:t>23 Mar</a:t>
+                      <a:t>24 Mar</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" sz="1800">
                       <a:solidFill>
@@ -5381,27 +5505,27 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="98" zoomScaleNormal="98" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25.33203125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="2.81640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.6328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.36328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.6328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.36328125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="201.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="201.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="178.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:1" ht="125.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:1" ht="178.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:1" ht="125.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5414,18 +5538,38 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1BDFFC7-2470-4DE4-A07A-1E31C9AD6941}">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="2:2" ht="30" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F0B35D7-F66F-4C4F-829A-963B3FBD2E66}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="2.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.81640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="2.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>10</v>
       </c>
@@ -5433,7 +5577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -5444,13 +5588,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="12" t="str">
         <f ca="1">IFERROR(IF(LEN('Chart Data'!B4)=0,"",IF('Chart Data'!$D$2="Year",YEAR('Chart Data'!B4),IF('Chart Data'!$D$2="Blank","",DAY('Chart Data'!B4)&amp;" "&amp;TEXT('Chart Data'!B4,"mmm")))),"")</f>
-        <v>8 Mar</v>
+        <v>9 Mar</v>
       </c>
       <c r="D3">
         <f ca="1">IFERROR(IF(LEN('Chart Data'!B4)=0,"",YEAR('Chart Data'!B4)),"")</f>
@@ -5460,13 +5604,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="12" t="str">
         <f ca="1">IFERROR(IF(LEN('Chart Data'!B5)=0,"",IF('Chart Data'!$D$2="Year",YEAR('Chart Data'!B5),IF('Chart Data'!$D$2="Blank","",DAY('Chart Data'!B5)&amp;" "&amp;TEXT('Chart Data'!B5,"mmm")))),"")</f>
-        <v>11 Mar</v>
+        <v>12 Mar</v>
       </c>
       <c r="D4">
         <f ca="1">IFERROR(IF(LEN('Chart Data'!B4)=0,"",IF(YEAR('Chart Data'!$B$6)=$D$3,$D$3,YEAR('Chart Data'!$B$6))),"")</f>
@@ -5476,13 +5620,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="12" t="str">
         <f ca="1">IFERROR(IF(LEN('Chart Data'!B6)=0,"",IF('Chart Data'!$D$2="Year",YEAR('Chart Data'!B6),IF('Chart Data'!$D$2="Blank","",DAY('Chart Data'!B6)&amp;" "&amp;TEXT('Chart Data'!B6,"mmm")))),"")</f>
-        <v>14 Mar</v>
+        <v>15 Mar</v>
       </c>
       <c r="D5" t="str">
         <f ca="1">IFERROR(IF(LEN('Chart Data'!B4)=0,"",IF(YEAR('Chart Data'!$B$9)=$D$3,"",YEAR('Chart Data'!$B$9))),"")</f>
@@ -5492,16 +5636,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="12" t="str">
         <f ca="1">IFERROR(IF(LEN('Chart Data'!B7)=0,"",IF('Chart Data'!$D$2="Year",YEAR('Chart Data'!B7),IF('Chart Data'!$D$2="Blank","",DAY('Chart Data'!B7)&amp;" "&amp;TEXT('Chart Data'!B7,"mmm")))),"")</f>
-        <v>17 Mar</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>18 Mar</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="12" t="str">
         <f ca="1">IFERROR(IF(LEN('Chart Data'!B9)=0,"",IF('Chart Data'!$D$2="Year",YEAR('Chart Data'!B9),IF('Chart Data'!$D$2="Blank","",DAY('Chart Data'!B9)&amp;" "&amp;TEXT('Chart Data'!B9,"mmm")))),"")</f>
-        <v>23 Mar</v>
+        <v>24 Mar</v>
       </c>
     </row>
   </sheetData>
@@ -5530,18 +5674,18 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="30.77734375" customWidth="1"/>
-    <col min="5" max="5" width="47.5546875" customWidth="1"/>
+    <col min="1" max="1" width="2.81640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" customWidth="1"/>
+    <col min="3" max="3" width="20.36328125" customWidth="1"/>
+    <col min="4" max="4" width="30.81640625" customWidth="1"/>
+    <col min="5" max="5" width="47.54296875" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" customWidth="1"/>
+    <col min="7" max="7" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>15</v>
       </c>
@@ -5549,17 +5693,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
       <c r="D2" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>18</v>
       </c>
@@ -5582,13 +5726,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="8">
         <f ca="1">TODAY()+10</f>
-        <v>43532</v>
+        <v>43533</v>
       </c>
       <c r="C4" t="s">
         <v>36</v>
@@ -5606,10 +5750,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="157.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="150" x14ac:dyDescent="0.35">
       <c r="B5" s="8">
         <f ca="1">B4+3</f>
-        <v>43535</v>
+        <v>43536</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
@@ -5627,10 +5771,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B6" s="8">
         <f ca="1">B5+3</f>
-        <v>43538</v>
+        <v>43539</v>
       </c>
       <c r="C6" t="s">
         <v>35</v>
@@ -5644,10 +5788,10 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B7" s="8">
         <f ca="1">B6+3</f>
-        <v>43541</v>
+        <v>43542</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -5661,10 +5805,10 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B8" s="8">
         <f ca="1">B7+3</f>
-        <v>43544</v>
+        <v>43545</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>32</v>
@@ -5678,10 +5822,10 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B9" s="8">
         <f ca="1">B8+3</f>
-        <v>43547</v>
+        <v>43548</v>
       </c>
       <c r="C9" t="s">
         <v>40</v>
@@ -5693,7 +5837,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B12" t="str">
         <f ca="1">TEXT(B4,"mmm")</f>
         <v>Mar</v>
@@ -5728,27 +5872,27 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="78.77734375" customWidth="1"/>
+    <col min="1" max="1" width="78.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.4">
       <c r="A4" s="7"/>
     </row>
   </sheetData>
@@ -5762,24 +5906,187 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFF4BA9-4330-4B94-98EA-9AE5DB38B034}">
-  <dimension ref="B2:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D3CEFA-066B-4175-B68B-3BD82EB48E2A}">
+  <dimension ref="B2:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="29.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" customWidth="1"/>
+    <col min="4" max="4" width="43.6328125" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="21"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="63" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>102</v>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B2" s="21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="30" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="30" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>118</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -5788,21 +6095,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFF2CEA6-C1B8-4777-AD41-56DD4A82F4D9}">
-  <dimension ref="B2:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFF4BA9-4330-4B94-98EA-9AE5DB38B034}">
+  <dimension ref="B2:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="63" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" ht="60" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -5811,6 +6124,32 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFF2CEA6-C1B8-4777-AD41-56DD4A82F4D9}">
+  <dimension ref="B2:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="2:5" ht="60" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA92F18-346F-4F83-B262-F4BCE4A3F213}">
   <dimension ref="B2:H14"/>
   <sheetViews>
@@ -5818,14 +6157,14 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.08984375" customWidth="1"/>
+    <col min="3" max="3" width="10.36328125" customWidth="1"/>
+    <col min="4" max="4" width="16.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" s="14" t="s">
         <v>73</v>
       </c>
@@ -5846,7 +6185,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="30" x14ac:dyDescent="0.35">
       <c r="B3" s="13" t="s">
         <v>47</v>
       </c>
@@ -5863,7 +6202,7 @@
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
         <v>53</v>
       </c>
@@ -5880,7 +6219,7 @@
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="30" x14ac:dyDescent="0.35">
       <c r="B5" s="13" t="s">
         <v>54</v>
       </c>
@@ -5901,7 +6240,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="30" x14ac:dyDescent="0.35">
       <c r="B6" s="13" t="s">
         <v>56</v>
       </c>
@@ -5922,7 +6261,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" ht="30" x14ac:dyDescent="0.35">
       <c r="B7" s="13" t="s">
         <v>58</v>
       </c>
@@ -5943,7 +6282,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" ht="30" x14ac:dyDescent="0.35">
       <c r="B8" s="13" t="s">
         <v>59</v>
       </c>
@@ -5964,7 +6303,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" ht="30" x14ac:dyDescent="0.35">
       <c r="B9" s="13" t="s">
         <v>63</v>
       </c>
@@ -5985,7 +6324,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="30" x14ac:dyDescent="0.35">
       <c r="B10" s="13" t="s">
         <v>64</v>
       </c>
@@ -6006,7 +6345,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" ht="30" x14ac:dyDescent="0.35">
       <c r="B11" s="13" t="s">
         <v>65</v>
       </c>
@@ -6027,7 +6366,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.35">
       <c r="B12" s="13" t="s">
         <v>66</v>
       </c>
@@ -6048,7 +6387,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" ht="30" x14ac:dyDescent="0.35">
       <c r="B13" s="13" t="s">
         <v>67</v>
       </c>
@@ -6069,7 +6408,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.35">
       <c r="B14" s="13" t="s">
         <v>68</v>
       </c>
@@ -6096,7 +6435,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F30FB23-F547-477F-937C-322AE94B0FCA}">
   <dimension ref="B1:H12"/>
   <sheetViews>
@@ -6104,12 +6443,12 @@
       <selection activeCell="H11" sqref="B1:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B1" s="14" t="s">
         <v>73</v>
       </c>
@@ -6130,7 +6469,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="30" x14ac:dyDescent="0.35">
       <c r="B2" s="13" t="s">
         <v>72</v>
       </c>
@@ -6147,7 +6486,7 @@
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
     </row>
-    <row r="3" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="30" x14ac:dyDescent="0.35">
       <c r="B3" s="13" t="s">
         <v>79</v>
       </c>
@@ -6162,7 +6501,7 @@
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
@@ -6171,7 +6510,7 @@
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="30" x14ac:dyDescent="0.35">
       <c r="B5" s="16" t="s">
         <v>78</v>
       </c>
@@ -6190,7 +6529,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="30" x14ac:dyDescent="0.35">
       <c r="B6" s="17" t="s">
         <v>84</v>
       </c>
@@ -6209,7 +6548,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" ht="30" x14ac:dyDescent="0.35">
       <c r="B7" s="13" t="s">
         <v>86</v>
       </c>
@@ -6228,7 +6567,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" ht="30" x14ac:dyDescent="0.35">
       <c r="B8" s="13" t="s">
         <v>89</v>
       </c>
@@ -6247,7 +6586,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="78.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" ht="75" x14ac:dyDescent="0.35">
       <c r="B9" s="18" t="s">
         <v>90</v>
       </c>
@@ -6268,7 +6607,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="30" x14ac:dyDescent="0.35">
       <c r="B10" s="18" t="s">
         <v>91</v>
       </c>
@@ -6287,7 +6626,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" ht="30" x14ac:dyDescent="0.35">
       <c r="B11" s="13" t="s">
         <v>96</v>
       </c>
@@ -6306,7 +6645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
     </row>
@@ -6315,7 +6654,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D28D24-6CA4-446D-AE67-FF7BE57861B4}">
   <dimension ref="B2"/>
   <sheetViews>
@@ -6323,29 +6662,9 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:2" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1BDFFC7-2470-4DE4-A07A-1E31C9AD6941}">
-  <dimension ref="B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="2" spans="2:2" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" ht="30" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
wording changed for better understand.
</commit_message>
<xml_diff>
--- a/Milestones.xlsx
+++ b/Milestones.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunny\Desktop\Betty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7611E4A4-DC40-432B-A190-5B75578BB52E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F701B6FE-8C70-4F59-87C2-79675AE3C178}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{3061E5F0-7863-451F-8C41-DAF595B62750}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3061E5F0-7863-451F-8C41-DAF595B62750}"/>
   </bookViews>
   <sheets>
-    <sheet name="Infographic Timeline" sheetId="2" r:id="rId1"/>
+    <sheet name=" Timeline" sheetId="2" r:id="rId1"/>
     <sheet name="Chart Data" sheetId="1" r:id="rId2"/>
     <sheet name="About" sheetId="3" r:id="rId3"/>
     <sheet name="LTS-6 Loads in excel sheet" sheetId="11" r:id="rId4"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="144">
   <si>
     <t>Date</t>
   </si>
@@ -143,9 +143,6 @@
     <t xml:space="preserve">scope of works and description </t>
   </si>
   <si>
-    <t>VBA file or excel file, or crystal report file or ssrp file, which will require least installation from customer.</t>
-  </si>
-  <si>
     <t>msexcel file and msword files should be able to get the name from data_collected_fieldsnotes.xlsx</t>
   </si>
   <si>
@@ -155,9 +152,6 @@
     <t>retest and code review</t>
   </si>
   <si>
-    <t>worker provide, from the data file: data_collected_fieldsnotes.xlsx, input into calculation data processing file, and run the calculation inside excel files  excel file will do odbc connection to data file and read the data out, and put into calculation, and , verify if the result files and folder exist, if yes, skip the row, and jump to next row, if not create the files and folders and conduct the calculation and transfer the result to the word file and also append self to the word files and save as word file and on the screen show the progress bar indicate the progress.</t>
-  </si>
-  <si>
     <t>process data</t>
   </si>
   <si>
@@ -437,49 +431,107 @@
     <t xml:space="preserve">data_collected_fieldsnotes: SHEET1: </t>
   </si>
   <si>
-    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$B$2</t>
-  </si>
-  <si>
-    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$C$2</t>
-  </si>
-  <si>
-    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$D$2</t>
-  </si>
-  <si>
     <t>C224</t>
   </si>
   <si>
-    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$e$2</t>
-  </si>
-  <si>
-    <t>data_collected_fieldsnotes.xlsx]reportinfo!$F$2</t>
-  </si>
-  <si>
-    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$G$2</t>
-  </si>
-  <si>
-    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$h$2</t>
-  </si>
-  <si>
-    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$I$2</t>
-  </si>
-  <si>
-    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$J$2</t>
-  </si>
-  <si>
-    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$K$2</t>
-  </si>
-  <si>
-    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$M$2</t>
-  </si>
-  <si>
-    <t>[data_collected_fieldsnotes.xlsx]reportinfo!$L$2</t>
-  </si>
-  <si>
     <t>foundation depth</t>
   </si>
   <si>
-    <t>only first sheet: LTS-6 LOADS take input rom data files data_collected_fieldsnotes.xlsx</t>
+    <t>refer the readme.pdf file for the function this need to perform.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VBA file or excel file, or crystal report file or ssrp file, which will require least installation from customer. </t>
+  </si>
+  <si>
+    <t>only first sheet: LTS-6 LOADS take input rom data files data</t>
+  </si>
+  <si>
+    <t>[data]reportinfo!$B$2</t>
+  </si>
+  <si>
+    <t>[data]reportinfo!$C$2</t>
+  </si>
+  <si>
+    <t>[data]reportinfo!$D$2</t>
+  </si>
+  <si>
+    <t>[data]reportinfo!$e$2</t>
+  </si>
+  <si>
+    <t>data]reportinfo!$F$2</t>
+  </si>
+  <si>
+    <t>[data]reportinfo!$G$2</t>
+  </si>
+  <si>
+    <t>[data]reportinfo!$h$2</t>
+  </si>
+  <si>
+    <t>[data]reportinfo!$I$2</t>
+  </si>
+  <si>
+    <t>[data]reportinfo!$J$2</t>
+  </si>
+  <si>
+    <t>[data]reportinfo!$K$2</t>
+  </si>
+  <si>
+    <t>[data]reportinfo!$L$2</t>
+  </si>
+  <si>
+    <t>[data]reportinfo!$M$2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This sheet is from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calc_template.xlsx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    :Constrained Foundation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This sheet is from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calc_template.xlsx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    :   nonConstrained Foundation</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -682,14 +734,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -817,8 +869,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="347993" y="143886"/>
-          <a:ext cx="9932008" cy="6548457"/>
+          <a:off x="349898" y="145791"/>
+          <a:ext cx="10114772" cy="6564085"/>
           <a:chOff x="349898" y="349898"/>
           <a:chExt cx="10114772" cy="6564085"/>
         </a:xfrm>
@@ -3334,7 +3386,7 @@
                         <a:latin typeface="Franklin Gothic Book"/>
                       </a:rPr>
                       <a:pPr algn="ctr"/>
-                      <a:t>9 Mar</a:t>
+                      <a:t>1 Mar</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" sz="1200">
                       <a:solidFill>
@@ -3643,7 +3695,7 @@
                         <a:latin typeface="Franklin Gothic Book"/>
                       </a:rPr>
                       <a:pPr algn="ctr"/>
-                      <a:t>12 Mar</a:t>
+                      <a:t>4 Mar</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" sz="1300">
                       <a:solidFill>
@@ -3949,7 +4001,7 @@
                         <a:latin typeface="Franklin Gothic Book"/>
                       </a:rPr>
                       <a:pPr algn="ctr"/>
-                      <a:t>15 Mar</a:t>
+                      <a:t>7 Mar</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" sz="1500">
                       <a:solidFill>
@@ -4255,7 +4307,7 @@
                         <a:latin typeface="Franklin Gothic Book"/>
                       </a:rPr>
                       <a:pPr algn="ctr"/>
-                      <a:t>18 Mar</a:t>
+                      <a:t>10 Mar</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" sz="1500">
                       <a:solidFill>
@@ -4561,7 +4613,7 @@
                         <a:latin typeface="Franklin Gothic Book"/>
                       </a:rPr>
                       <a:pPr algn="ctr"/>
-                      <a:t>24 Mar</a:t>
+                      <a:t>16 Mar</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US" sz="1800">
                       <a:solidFill>
@@ -5505,27 +5557,29 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="98" zoomScaleNormal="98" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="16.81640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.6328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.36328125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25.36328125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.90625" style="2"/>
+    <col min="1" max="1" width="2.77734375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.33203125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="201.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="201.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="178.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:1" ht="125.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:1" ht="178.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:1" ht="125.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5542,14 +5596,14 @@
   <dimension ref="B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:2" ht="30" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -5563,13 +5617,13 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="2.81640625" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="2.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>10</v>
       </c>
@@ -5577,7 +5631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -5588,64 +5642,64 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="12" t="str">
-        <f ca="1">IFERROR(IF(LEN('Chart Data'!B4)=0,"",IF('Chart Data'!$D$2="Year",YEAR('Chart Data'!B4),IF('Chart Data'!$D$2="Blank","",DAY('Chart Data'!B4)&amp;" "&amp;TEXT('Chart Data'!B4,"mmm")))),"")</f>
-        <v>9 Mar</v>
+        <f>IFERROR(IF(LEN('Chart Data'!B4)=0,"",IF('Chart Data'!$D$2="Year",YEAR('Chart Data'!B4),IF('Chart Data'!$D$2="Blank","",DAY('Chart Data'!B4)&amp;" "&amp;TEXT('Chart Data'!B4,"mmm")))),"")</f>
+        <v>1 Mar</v>
       </c>
       <c r="D3">
-        <f ca="1">IFERROR(IF(LEN('Chart Data'!B4)=0,"",YEAR('Chart Data'!B4)),"")</f>
+        <f>IFERROR(IF(LEN('Chart Data'!B4)=0,"",YEAR('Chart Data'!B4)),"")</f>
         <v>2019</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="12" t="str">
-        <f ca="1">IFERROR(IF(LEN('Chart Data'!B5)=0,"",IF('Chart Data'!$D$2="Year",YEAR('Chart Data'!B5),IF('Chart Data'!$D$2="Blank","",DAY('Chart Data'!B5)&amp;" "&amp;TEXT('Chart Data'!B5,"mmm")))),"")</f>
-        <v>12 Mar</v>
+        <f>IFERROR(IF(LEN('Chart Data'!B5)=0,"",IF('Chart Data'!$D$2="Year",YEAR('Chart Data'!B5),IF('Chart Data'!$D$2="Blank","",DAY('Chart Data'!B5)&amp;" "&amp;TEXT('Chart Data'!B5,"mmm")))),"")</f>
+        <v>4 Mar</v>
       </c>
       <c r="D4">
-        <f ca="1">IFERROR(IF(LEN('Chart Data'!B4)=0,"",IF(YEAR('Chart Data'!$B$6)=$D$3,$D$3,YEAR('Chart Data'!$B$6))),"")</f>
+        <f>IFERROR(IF(LEN('Chart Data'!B4)=0,"",IF(YEAR('Chart Data'!$B$6)=$D$3,$D$3,YEAR('Chart Data'!$B$6))),"")</f>
         <v>2019</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="12" t="str">
-        <f ca="1">IFERROR(IF(LEN('Chart Data'!B6)=0,"",IF('Chart Data'!$D$2="Year",YEAR('Chart Data'!B6),IF('Chart Data'!$D$2="Blank","",DAY('Chart Data'!B6)&amp;" "&amp;TEXT('Chart Data'!B6,"mmm")))),"")</f>
-        <v>15 Mar</v>
+        <f>IFERROR(IF(LEN('Chart Data'!B6)=0,"",IF('Chart Data'!$D$2="Year",YEAR('Chart Data'!B6),IF('Chart Data'!$D$2="Blank","",DAY('Chart Data'!B6)&amp;" "&amp;TEXT('Chart Data'!B6,"mmm")))),"")</f>
+        <v>7 Mar</v>
       </c>
       <c r="D5" t="str">
-        <f ca="1">IFERROR(IF(LEN('Chart Data'!B4)=0,"",IF(YEAR('Chart Data'!$B$9)=$D$3,"",YEAR('Chart Data'!$B$9))),"")</f>
+        <f>IFERROR(IF(LEN('Chart Data'!B4)=0,"",IF(YEAR('Chart Data'!$B$9)=$D$3,"",YEAR('Chart Data'!$B$9))),"")</f>
         <v/>
       </c>
       <c r="E5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="str">
-        <f ca="1">IFERROR(IF(LEN('Chart Data'!B7)=0,"",IF('Chart Data'!$D$2="Year",YEAR('Chart Data'!B7),IF('Chart Data'!$D$2="Blank","",DAY('Chart Data'!B7)&amp;" "&amp;TEXT('Chart Data'!B7,"mmm")))),"")</f>
-        <v>18 Mar</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <f>IFERROR(IF(LEN('Chart Data'!B7)=0,"",IF('Chart Data'!$D$2="Year",YEAR('Chart Data'!B7),IF('Chart Data'!$D$2="Blank","",DAY('Chart Data'!B7)&amp;" "&amp;TEXT('Chart Data'!B7,"mmm")))),"")</f>
+        <v>10 Mar</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="str">
-        <f ca="1">IFERROR(IF(LEN('Chart Data'!B9)=0,"",IF('Chart Data'!$D$2="Year",YEAR('Chart Data'!B9),IF('Chart Data'!$D$2="Blank","",DAY('Chart Data'!B9)&amp;" "&amp;TEXT('Chart Data'!B9,"mmm")))),"")</f>
-        <v>24 Mar</v>
+        <f>IFERROR(IF(LEN('Chart Data'!B9)=0,"",IF('Chart Data'!$D$2="Year",YEAR('Chart Data'!B9),IF('Chart Data'!$D$2="Blank","",DAY('Chart Data'!B9)&amp;" "&amp;TEXT('Chart Data'!B9,"mmm")))),"")</f>
+        <v>16 Mar</v>
       </c>
     </row>
   </sheetData>
@@ -5671,21 +5725,21 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="16.36328125" customWidth="1"/>
-    <col min="3" max="3" width="20.36328125" customWidth="1"/>
-    <col min="4" max="4" width="30.81640625" customWidth="1"/>
-    <col min="5" max="5" width="47.54296875" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.77734375" customWidth="1"/>
+    <col min="5" max="5" width="47.5546875" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="21.453125" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>15</v>
       </c>
@@ -5693,17 +5747,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
       <c r="D2" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="31.5" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>18</v>
       </c>
@@ -5726,16 +5780,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="31.5" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="8">
-        <f ca="1">TODAY()+10</f>
-        <v>43533</v>
+        <v>43525</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
@@ -5750,96 +5803,96 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="150" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="94.5" x14ac:dyDescent="0.3">
       <c r="B5" s="8">
-        <f ca="1">B4+3</f>
-        <v>43536</v>
+        <f>B4+3</f>
+        <v>43528</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="8">
+        <f>B5+3</f>
+        <v>43531</v>
+      </c>
+      <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B6" s="8">
-        <f ca="1">B5+3</f>
-        <v>43539</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="8">
-        <f ca="1">B6+3</f>
-        <v>43542</v>
+        <f>B6+3</f>
+        <v>43534</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="8">
-        <f ca="1">B7+3</f>
-        <v>43545</v>
+        <f>B7+3</f>
+        <v>43537</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="8">
-        <f ca="1">B8+3</f>
-        <v>43548</v>
+        <f>B8+3</f>
+        <v>43540</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
-        <f ca="1">TEXT(B4,"mmm")</f>
+        <f>TEXT(B4,"mmm")</f>
         <v>Mar</v>
       </c>
     </row>
@@ -5872,27 +5925,27 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="78.81640625" customWidth="1"/>
+    <col min="1" max="1" width="78.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
     </row>
   </sheetData>
@@ -5909,184 +5962,184 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D3CEFA-066B-4175-B68B-3BD82EB48E2A}">
   <dimension ref="B2:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="15.36328125" customWidth="1"/>
-    <col min="4" max="4" width="43.6328125" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="21"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="43.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" style="20"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B2" s="21" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="31.5" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="31.5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="47.25" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" ht="30" x14ac:dyDescent="0.35">
-      <c r="D3" t="s">
+      <c r="C5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" s="20" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="30" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F18" s="20" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C9" t="s">
-        <v>110</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C12" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C13" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C14" t="s">
-        <v>115</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C15" t="s">
-        <v>116</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C16" t="s">
-        <v>117</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C17" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="F17" s="21" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C18" t="s">
-        <v>130</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -6096,52 +6149,63 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFF4BA9-4330-4B94-98EA-9AE5DB38B034}">
-  <dimension ref="B2:E2"/>
+  <dimension ref="B1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="60" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="20" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" ht="63" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFF2CEA6-C1B8-4777-AD41-56DD4A82F4D9}">
-  <dimension ref="B2:E2"/>
+  <dimension ref="B1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:5" ht="60" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:5" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="20" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" ht="63" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C2" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" t="s">
         <v>101</v>
-      </c>
-      <c r="E2" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -6157,273 +6221,273 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.08984375" customWidth="1"/>
-    <col min="3" max="3" width="10.36328125" customWidth="1"/>
-    <col min="4" max="4" width="16.36328125" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E2" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" ht="30" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B3" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>48</v>
-      </c>
       <c r="F3" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>50</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>52</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="2:8" ht="30" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B5" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H5" s="13">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" s="13">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="30" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B7" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H7" s="13">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="30" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B8" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H8" s="13">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="30" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B9" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H9" s="13">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="30" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B10" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H10" s="13">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="30" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B11" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H11" s="13">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B12" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H12" s="13">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="30" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B13" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H13" s="13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B14" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H14" s="13">
         <v>12</v>
@@ -6443,65 +6507,65 @@
       <selection activeCell="H11" sqref="B1:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.08984375" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B1" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8" ht="30" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B2" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
     </row>
-    <row r="3" spans="2:8" ht="30" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B3" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
@@ -6510,142 +6574,142 @@
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="2:8" ht="30" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B5" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H5" s="13">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B6" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" s="13">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="30" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B7" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H7" s="13">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="30" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B8" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H8" s="13">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="75" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="78.75" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E9" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>94</v>
-      </c>
       <c r="G9" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H9" s="13">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="30" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H10" s="13">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="30" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B11" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H11" s="13">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
     </row>
@@ -6662,11 +6726,11 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:2" ht="30" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2" ht="31.5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>